<commit_message>
main flowchart updated & completed, successfully triained ML AI model sentiment analysis in our application using AI Centre in UiPath
</commit_message>
<xml_diff>
--- a/Output/ShoppingListForm.xlsx
+++ b/Output/ShoppingListForm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cyan\Documents\UiPath\Newfolder\AIPriceComparisonApp\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E79AA67-52CF-4039-8897-0C941414F387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D5B7CC-1E71-4E74-B351-8ECF8E3221EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1725" windowWidth="28110" windowHeight="16440" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="20910" windowHeight="11835" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="99">
   <si>
     <t>Name</t>
   </si>
@@ -111,7 +111,7 @@
     <t>Alice_Aw's Market Fresh Indonesian Pork Belly (Sliced)</t>
   </si>
   <si>
-    <t>https://www.fairprice.com.sg/product/aw-s-market-fresh-indonesian-pork-belly-sliced-250-g-90018587</t>
+    <t>https://www.fairprice.com.sg/search?query=Aw%27s%20Market%20Fresh%20Indonesian%20Pork%20Belly%20(Sliced)</t>
   </si>
   <si>
     <t>$6.00</t>
@@ -144,7 +144,7 @@
     <t>Bruce_Pokka Ice Lemon Tea</t>
   </si>
   <si>
-    <t>https://www.fairprice.com.sg/product/pokka-ice-lemon-tea-15lt-376287</t>
+    <t>https://www.fairprice.com.sg/search?query=Pokka%20Ice%20Lemon%20Tea</t>
   </si>
   <si>
     <t>$2.15</t>
@@ -159,13 +159,13 @@
     <t>Bruce_Ruffles Chicken</t>
   </si>
   <si>
-    <t>https://www.fairprice.com.sg/product/aw-s-market-chicken-breast-skinless-200-g-90134679</t>
-  </si>
-  <si>
-    <t>$3.50</t>
-  </si>
-  <si>
-    <t>3.5</t>
+    <t>https://www.fairprice.com.sg/product/ruffles-potato-chips-chicken-184-2g-13086598</t>
+  </si>
+  <si>
+    <t>$5.30</t>
+  </si>
+  <si>
+    <t>5.3</t>
   </si>
   <si>
     <t>Wayne</t>
@@ -177,7 +177,7 @@
     <t>Wayne_Marigold HL Milk - Chocolate</t>
   </si>
   <si>
-    <t>https://www.fairprice.com.sg/product/marigold-hl-milk-chocolate-1lt-10054432</t>
+    <t>https://www.fairprice.com.sg/search?query=Marigold%20HL%20Milk%20-%20Chocolate</t>
   </si>
   <si>
     <t>$3.53</t>
@@ -240,7 +240,7 @@
     <t>George_Lipton Yellow Label Tea</t>
   </si>
   <si>
-    <t>https://www.fairprice.com.sg/product/lipton-yellow-label-teabags-100s-72207</t>
+    <t>https://www.fairprice.com.sg/search?query=Lipton%20Yellow%20Label%20Tea</t>
   </si>
   <si>
     <t>$5.70</t>
@@ -255,7 +255,7 @@
     <t>George_Panteen Shampoo Hail Fall Control</t>
   </si>
   <si>
-    <t>https://www.fairprice.com.sg/product/pantene-shampoo-hair-fall-control-680ml-13194383</t>
+    <t>https://www.fairprice.com.sg/search?query=Panteen%20Shampoo%20Hail%20Fall%20Control</t>
   </si>
   <si>
     <t>$11.61</t>
@@ -373,9 +373,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -736,7 +735,7 @@
         <v>3.99</v>
       </c>
       <c r="J2">
-        <v>14.99</v>
+        <v>22.52</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -814,7 +813,7 @@
         <v>3.99</v>
       </c>
       <c r="J5">
-        <v>26.49</v>
+        <v>28.29</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1025,130 +1024,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A05DAFD9-A3F9-4953-BE96-F81EED202324}">
-  <dimension ref="A1:J4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="2">
-        <v>3.9</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>3.9</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>3.99</v>
-      </c>
-      <c r="J2">
-        <v>14.99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2">
-        <v>3.63</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>3.63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="2">
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E5ACEE-EA76-4E25-8B10-BECB0471869B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3AB212-992E-4659-9FA2-6E35086BAF8F}">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1183,19 +1059,19 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="3">
-        <v>4.95</v>
+        <v>94</v>
+      </c>
+      <c r="B2">
+        <v>3.95</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="E2">
-        <v>4.95</v>
+        <v>3.95</v>
       </c>
       <c r="F2">
         <v>6</v>
@@ -1209,36 +1085,36 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="3">
-        <v>2.15</v>
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>3.6</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="E3">
-        <v>2.15</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="3">
-        <v>4.75</v>
+        <v>97</v>
+      </c>
+      <c r="B4">
+        <v>4.45</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="E4">
-        <v>4.75</v>
+        <v>4.45</v>
       </c>
     </row>
   </sheetData>
@@ -1246,8 +1122,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C483800-40BF-4B7E-A997-8706BC1BF67E}">
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15B4824F-1615-48BC-964C-4E1898C2DA7C}">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1282,6 +1158,105 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4.95</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2">
+        <v>4.95</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>1.99</v>
+      </c>
+      <c r="H2">
+        <v>19.989999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2.15</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4.75</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4">
+        <v>4.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE7A362-EE31-4C8E-930F-408A2D5A88C9}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>84</v>
       </c>
       <c r="B2">
@@ -1346,7 +1321,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68525EA9-D39C-4D8D-B9B3-96DFB39BB98C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC7A689E-CA86-4DCE-8B34-BE6775A4A4DF}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1398,7 +1373,7 @@
       <c r="D2" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>3.33</v>
       </c>
       <c r="F2">
@@ -1430,7 +1405,7 @@
       <c r="D3" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>5.7</v>
       </c>
       <c r="F3">
@@ -1453,7 +1428,7 @@
       <c r="D4" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>11.61</v>
       </c>
       <c r="F4">
@@ -1886,7 +1861,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E997B2-C8B7-4F8C-A5AC-2A046E6666FA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F24B7D-969D-43A3-A478-C971577EB681}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1954,7 +1929,7 @@
         <v>3.99</v>
       </c>
       <c r="J2">
-        <v>14.99</v>
+        <v>22.52</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2009,7 +1984,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B244952B-EB54-440E-85A5-F654A01A8BB3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D39F3D8D-CE0B-4645-9ECD-02213DD50B24}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2077,7 +2052,7 @@
         <v>3.99</v>
       </c>
       <c r="J2">
-        <v>26.49</v>
+        <v>28.29</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2117,13 +2092,13 @@
         <v>40</v>
       </c>
       <c r="E4" s="1">
-        <v>3.5</v>
+        <v>5.3</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>3.5</v>
+        <v>5.3</v>
       </c>
     </row>
   </sheetData>
@@ -2132,7 +2107,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6042328-8B27-43A0-A203-E49EAE18C35F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453A66F3-A4DA-4F19-B809-FE1E260A31E6}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2255,7 +2230,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6458C7-4FC0-47EE-B074-083E92F0BD83}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED184B4D-E201-4461-A5E4-22FA861A5D1C}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>